<commit_message>
refactor some var name
</commit_message>
<xml_diff>
--- a/action.xlsx
+++ b/action.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64\home\win10\project\SekiroAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208EB071-4B16-4EEB-A177-BE876DC474B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8730CD21-9EBC-4B2F-BBA4-63378FB59A5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="npc action list" sheetId="1" r:id="rId1"/>
-    <sheet name="pc action group" sheetId="5" r:id="rId2"/>
-    <sheet name="pc action list" sheetId="6" r:id="rId3"/>
+    <sheet name="pc action list" sheetId="6" r:id="rId2"/>
+    <sheet name="pc action group" sheetId="5" r:id="rId3"/>
     <sheet name="tae block" sheetId="7" r:id="rId4"/>
     <sheet name="goal" sheetId="8" r:id="rId5"/>
     <sheet name="action state" sheetId="4" r:id="rId6"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="343">
   <si>
     <t>动作编号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1177,6 +1177,14 @@
   </si>
   <si>
     <t>idle to 右走</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可能 和ai state 相关</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>同 600，随机动作选择</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1539,8 +1547,8 @@
   <dimension ref="A1:G133"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1606,6 +1614,9 @@
       <c r="B5">
         <v>610</v>
       </c>
+      <c r="G5" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -2580,6 +2591,148 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22CDCB92-CE3E-45F7-A319-2A67B1B418BF}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>100</v>
+      </c>
+      <c r="B7" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>101</v>
+      </c>
+      <c r="B8" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>102</v>
+      </c>
+      <c r="B9" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>103</v>
+      </c>
+      <c r="B10" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ABB2919-42DE-487A-884A-9A2000FB0D8F}">
   <dimension ref="A1:C76"/>
   <sheetViews>
@@ -3048,148 +3201,6 @@
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>250</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22CDCB92-CE3E-45F7-A319-2A67B1B418BF}">
-  <dimension ref="A1:C18"/>
-  <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="12.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>330</v>
-      </c>
-      <c r="B1" t="s">
-        <v>331</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>100</v>
-      </c>
-      <c r="B7" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>101</v>
-      </c>
-      <c r="B8" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>102</v>
-      </c>
-      <c r="B9" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>103</v>
-      </c>
-      <c r="B10" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -3215,7 +3226,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30DF551E-091C-406A-B47E-9CF6E1DCAF3F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
@@ -3229,7 +3240,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3297,6 +3308,9 @@
       <c r="A12">
         <v>1</v>
       </c>
+      <c r="B12" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -3339,8 +3353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5677D762-D1D7-4829-8D49-2EA8BE920C39}">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>